<commit_message>
update the excel doc
</commit_message>
<xml_diff>
--- a/public/Note Templates.xlsx
+++ b/public/Note Templates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason-crmnext/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason-crmnext/Documents/crmnext/demoCaseNotes/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4946867A-321B-4E40-B2E2-92B95DA678B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DDB7B2-870A-BB4E-B1E8-851B000CD1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19620" xr2:uid="{31364E8F-0872-1F41-B8D0-461C835138D9}"/>
+    <workbookView xWindow="13540" yWindow="500" windowWidth="20060" windowHeight="19620" xr2:uid="{31364E8F-0872-1F41-B8D0-461C835138D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Type</t>
   </si>
@@ -82,7 +82,33 @@
     <t>Auto Loan</t>
   </si>
   <si>
-    <t>Auto Loan Demo</t>
+    <t>Disputed Debit Card Transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    &lt;h3&gt;&lt;u&gt;Debit Card Dispute&lt;/u&gt;&lt;/h3&gt;
+    1. Immediately block this card to prevent any further fraudulent charges.
+    &lt;br&gt;
+      &lt;br&gt;
+        2. Before submitting the dispute, ensure the customer/member has already called the merchant to inquire about the charge.
+        &lt;br&gt;
+          &lt;br&gt;
+            3. Inform customer/member it will take up to 10 business days to receive provisional credit for this charge
+            &lt;br&gt;
+              &lt;br&gt;
+                &lt;strong&gt;Links&lt;/strong&gt;
+                &lt;ul&gt;
+                  &lt;li&gt;&lt;a href="https://crmnext.us" target="_blank"&gt; Policy and Procedures Manual&lt;/a&gt;&lt;/li&gt;
+                  &lt;li&gt;&lt;a href="https://crmnext.us" target="_blank"&gt; Policy and Procedures Manual&lt;/a&gt;&lt;/li&gt;
+                  &lt;li&gt;&lt;a href="https://crmnext.us" target="_blank"&gt; Policy and Procedures Manual&lt;/a&gt;&lt;/li&gt;
+                  &lt;li&gt;&lt;a href="https://crmnext.us" target="_blank"&gt; Policy and Procedures Manual&lt;/a&gt;&lt;/li&gt;
+                &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;&lt;u&gt;Auto Loan&lt;/u&gt;&lt;/h3&gt;
+&lt;br&gt;
+&lt;br&gt;
+Steps to submit an auto loan!</t>
   </si>
 </sst>
 </file>
@@ -437,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CD0989-15D7-894A-8B8F-76B8508DC4DA}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,19 +498,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="404" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C3" xr:uid="{A0CD0989-15D7-894A-8B8F-76B8508DC4DA}"/>
+  <autoFilter ref="A1:C3" xr:uid="{A0CD0989-15D7-894A-8B8F-76B8508DC4DA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C4">
+      <sortCondition ref="A1:A4"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>